<commit_message>
Corrette section_id  a seguito segnalazione errori
GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\FSE test Infosys LDO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\FSE test Infosys LDO New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59FBFC5-F315-414D-AA21-C266F8B8D1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287752E0-6245-4DB0-B161-B44A08F657FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Summary" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhUlYP9yzNmk4f07XMJovPPUaqOhw=="/>
@@ -507,96 +507,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>2023-03-29T15:02:21.7000000Z</t>
-  </si>
-  <si>
-    <t>bb8b361ebb1c6246</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.88c7654e6a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:08:17.1866667Z</t>
-  </si>
-  <si>
-    <t>a47ba7ffb906ec33</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.f344827012^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:10:40.0933333Z</t>
-  </si>
-  <si>
-    <t>f7749537ad2c3b27</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.387e476585^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:12:35.6000000Z</t>
-  </si>
-  <si>
-    <t>43baf22fa414e882</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.6e37fc50f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:18:58.4133333Z</t>
-  </si>
-  <si>
-    <t>8672fd0a93fe4cdc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.bd54e5303f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:23:33.1800000Z</t>
-  </si>
-  <si>
-    <t>d2b140f0da72acf3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.95486f0ae1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:26:08.3000000Z</t>
-  </si>
-  <si>
-    <t>23f349a752c226a1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.33f07986e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:27:40.8366667Z</t>
-  </si>
-  <si>
-    <t>39519d3768876eb1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.990c5d5c26^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:29:21.6366667Z</t>
-  </si>
-  <si>
-    <t>ad27158c973e153f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.478ad1a8f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-29T15:30:44.1833333Z</t>
-  </si>
-  <si>
-    <t>67b6205c8af80d6e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.7f2edca41a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>L'applicativo gestisce alcune sezioni opzionali previste dal test solo come blocco narrativo e non come entry strutturate.</t>
   </si>
   <si>
@@ -680,6 +590,96 @@
   </si>
   <si>
     <t>subject_application_vendor: INFOSYS SRL</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:28:40.9466667Z</t>
+  </si>
+  <si>
+    <t>f5ea7021097667c7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.86a96fcf81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4e45e1bb08a02931</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:29:38.6100000Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.323f635787^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:30:47.6200000Z</t>
+  </si>
+  <si>
+    <t>8c1b523be4cec99b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.ce2cd4e448^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:31:44.6333333Z</t>
+  </si>
+  <si>
+    <t>01950dafafab4411</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.5293e67eeb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:32:22.6800000Z</t>
+  </si>
+  <si>
+    <t>655bcd391f15e583</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.792ff206e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:33:52.0300000Z</t>
+  </si>
+  <si>
+    <t>237ec6f0ab4a3d0f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.e3d22a7ff8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:34:24.5300000Z</t>
+  </si>
+  <si>
+    <t>40d47c9d21794879</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.34a912163b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:35:27.5800000Z</t>
+  </si>
+  <si>
+    <t>3cf928e430eac259</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.7527f66905^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T16:45:32.9366667Z</t>
+  </si>
+  <si>
+    <t>528e36d207d8f0b7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.e21c74eaf3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T17:36:05.0900000Z</t>
+  </si>
+  <si>
+    <t>c5ed6731d92de7f3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.209a55cdea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1090,6 +1090,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1114,18 +1126,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,17 +1448,17 @@
       </c>
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A4" s="46" t="s">
-        <v>125</v>
+      <c r="A4" s="33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="33" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3585,9 +3585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C453036-49B7-4D15-A5E1-2160AF8A9FAA}">
   <dimension ref="A1:T656"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3626,14 +3626,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="36"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="40"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3651,14 +3651,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="34"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="38"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3676,12 +3676,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="43" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="34"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="38"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3700,12 +3700,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="34"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="38"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3723,8 +3723,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -3858,16 +3858,16 @@
         <v>48</v>
       </c>
       <c r="F10" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G10" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" s="47" t="s">
-        <v>96</v>
+        <v>45027</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>121</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>60</v>
@@ -3908,9 +3908,9 @@
         <v>93</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="L11" s="45"/>
+        <v>94</v>
+      </c>
+      <c r="L11" s="32"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
@@ -3946,9 +3946,9 @@
         <v>93</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="L12" s="45"/>
+        <v>94</v>
+      </c>
+      <c r="L12" s="32"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
@@ -3984,7 +3984,7 @@
         <v>93</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -4017,27 +4017,27 @@
       <c r="F14" s="23">
         <v>45015</v>
       </c>
-      <c r="G14" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="47" t="s">
-        <v>139</v>
+      <c r="G14" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>109</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="O14" s="45" t="s">
+      <c r="N14" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="O14" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P14" s="45" t="s">
-        <v>144</v>
+      <c r="P14" s="32" t="s">
+        <v>114</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
@@ -4065,27 +4065,27 @@
       <c r="F15" s="23">
         <v>45015</v>
       </c>
-      <c r="G15" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="H15" s="47" t="s">
-        <v>143</v>
+      <c r="G15" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>113</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
-      <c r="N15" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="O15" s="45" t="s">
+      <c r="N15" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P15" s="45" t="s">
-        <v>144</v>
+      <c r="P15" s="32" t="s">
+        <v>114</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
@@ -4118,14 +4118,14 @@
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
-      <c r="N16" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="O16" s="45" t="s">
+      <c r="N16" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="O16" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P16" s="45" t="s">
-        <v>144</v>
+      <c r="P16" s="32" t="s">
+        <v>114</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4151,16 +4151,16 @@
         <v>63</v>
       </c>
       <c r="F17" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G17" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="47" t="s">
-        <v>99</v>
+        <v>45027</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>124</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>60</v>
@@ -4170,19 +4170,19 @@
       <c r="M17" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N17" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O17" s="45" t="s">
+      <c r="N17" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O17" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P17" s="45" t="s">
-        <v>138</v>
+      <c r="P17" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
-      <c r="S17" s="44" t="s">
-        <v>128</v>
+      <c r="S17" s="31" t="s">
+        <v>98</v>
       </c>
       <c r="T17" s="28" t="s">
         <v>44</v>
@@ -4205,16 +4205,16 @@
         <v>65</v>
       </c>
       <c r="F18" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="I18" s="47" t="s">
-        <v>102</v>
+        <v>45027</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>60</v>
@@ -4224,19 +4224,19 @@
       <c r="M18" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O18" s="45" t="s">
+      <c r="N18" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P18" s="45" t="s">
-        <v>138</v>
+      <c r="P18" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
-      <c r="S18" s="44" t="s">
-        <v>130</v>
+      <c r="S18" s="31" t="s">
+        <v>100</v>
       </c>
       <c r="T18" s="28" t="s">
         <v>44</v>
@@ -4259,16 +4259,16 @@
         <v>67</v>
       </c>
       <c r="F19" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="47" t="s">
-        <v>105</v>
+        <v>45027</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>130</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>60</v>
@@ -4278,19 +4278,19 @@
       <c r="M19" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N19" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O19" s="45" t="s">
+      <c r="N19" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O19" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P19" s="45" t="s">
-        <v>138</v>
+      <c r="P19" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
-      <c r="S19" s="44" t="s">
-        <v>129</v>
+      <c r="S19" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="T19" s="28" t="s">
         <v>44</v>
@@ -4313,16 +4313,16 @@
         <v>69</v>
       </c>
       <c r="F20" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G20" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20" s="47" t="s">
-        <v>108</v>
+        <v>45027</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>133</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>60</v>
@@ -4332,19 +4332,19 @@
       <c r="M20" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O20" s="45" t="s">
+      <c r="N20" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O20" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P20" s="45" t="s">
-        <v>138</v>
+      <c r="P20" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
-      <c r="S20" s="44" t="s">
-        <v>131</v>
+      <c r="S20" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="T20" s="28" t="s">
         <v>44</v>
@@ -4367,16 +4367,16 @@
         <v>71</v>
       </c>
       <c r="F21" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="47" t="s">
-        <v>111</v>
+        <v>45027</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>148</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>60</v>
@@ -4386,19 +4386,19 @@
       <c r="M21" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N21" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O21" s="45" t="s">
+      <c r="N21" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O21" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P21" s="45" t="s">
-        <v>138</v>
+      <c r="P21" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
-      <c r="S21" s="44" t="s">
-        <v>132</v>
+      <c r="S21" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="T21" s="28" t="s">
         <v>44</v>
@@ -4421,16 +4421,16 @@
         <v>73</v>
       </c>
       <c r="F22" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="I22" s="47" t="s">
-        <v>114</v>
+        <v>45027</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>136</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>60</v>
@@ -4440,19 +4440,19 @@
       <c r="M22" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N22" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O22" s="45" t="s">
+      <c r="N22" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O22" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="45" t="s">
-        <v>138</v>
+      <c r="P22" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
-      <c r="S22" s="44" t="s">
-        <v>133</v>
+      <c r="S22" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="T22" s="28" t="s">
         <v>44</v>
@@ -4475,16 +4475,16 @@
         <v>75</v>
       </c>
       <c r="F23" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23" s="47" t="s">
-        <v>117</v>
+        <v>45027</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>139</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>60</v>
@@ -4494,19 +4494,19 @@
       <c r="M23" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N23" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O23" s="45" t="s">
+      <c r="N23" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O23" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P23" s="45" t="s">
-        <v>138</v>
+      <c r="P23" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26"/>
-      <c r="S23" s="44" t="s">
-        <v>134</v>
+      <c r="S23" s="31" t="s">
+        <v>104</v>
       </c>
       <c r="T23" s="28" t="s">
         <v>44</v>
@@ -4529,16 +4529,16 @@
         <v>77</v>
       </c>
       <c r="F24" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="H24" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>120</v>
+        <v>45027</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>142</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>60</v>
@@ -4548,19 +4548,19 @@
       <c r="M24" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N24" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O24" s="45" t="s">
+      <c r="N24" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O24" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P24" s="45" t="s">
-        <v>138</v>
+      <c r="P24" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="26"/>
-      <c r="S24" s="44" t="s">
-        <v>135</v>
+      <c r="S24" s="31" t="s">
+        <v>105</v>
       </c>
       <c r="T24" s="28" t="s">
         <v>44</v>
@@ -4590,7 +4590,7 @@
         <v>93</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -4628,7 +4628,7 @@
         <v>93</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -4659,16 +4659,16 @@
         <v>83</v>
       </c>
       <c r="F27" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="H27" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="I27" s="47" t="s">
-        <v>123</v>
+        <v>45027</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>145</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>60</v>
@@ -4678,19 +4678,19 @@
       <c r="M27" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="O27" s="45" t="s">
+      <c r="N27" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O27" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="P27" s="45" t="s">
-        <v>138</v>
+      <c r="P27" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
-      <c r="S27" s="44" t="s">
-        <v>136</v>
+      <c r="S27" s="31" t="s">
+        <v>106</v>
       </c>
       <c r="T27" s="28" t="s">
         <v>44</v>
@@ -4720,7 +4720,7 @@
         <v>93</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>

</xml_diff>

<commit_message>
Aggiornamento report-checklist, fix campi mancanti
GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2

Correzione errori segnalati, integrati campi mancanti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\FSE test Infosys LDO New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287752E0-6245-4DB0-B161-B44A08F657FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B41C52-2C2C-446D-AFFA-E6E19758C4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Summary" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhUlYP9yzNmk4f07XMJovPPUaqOhw=="/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="149">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3583,11 +3583,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C453036-49B7-4D15-A5E1-2160AF8A9FAA}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:T656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -4026,10 +4029,16 @@
       <c r="I14" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
+      <c r="L14" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="N14" s="32" t="s">
         <v>115</v>
       </c>
@@ -4074,10 +4083,16 @@
       <c r="I15" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
+      <c r="L15" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="N15" s="32" t="s">
         <v>115</v>
       </c>
@@ -4114,15 +4129,21 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="J16" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="N16" s="32" t="s">
         <v>116</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="P16" s="32" t="s">
         <v>114</v>
@@ -4166,7 +4187,9 @@
         <v>60</v>
       </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M17" s="25" t="s">
         <v>60</v>
       </c>
@@ -4220,7 +4243,9 @@
         <v>60</v>
       </c>
       <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="L18" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M18" s="25" t="s">
         <v>60</v>
       </c>
@@ -4274,7 +4299,9 @@
         <v>60</v>
       </c>
       <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="L19" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M19" s="25" t="s">
         <v>60</v>
       </c>
@@ -4328,7 +4355,9 @@
         <v>60</v>
       </c>
       <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="L20" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M20" s="25" t="s">
         <v>60</v>
       </c>
@@ -4382,7 +4411,9 @@
         <v>60</v>
       </c>
       <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="L21" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M21" s="25" t="s">
         <v>60</v>
       </c>
@@ -4436,7 +4467,9 @@
         <v>60</v>
       </c>
       <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="L22" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M22" s="25" t="s">
         <v>60</v>
       </c>
@@ -4490,7 +4523,9 @@
         <v>60</v>
       </c>
       <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
+      <c r="L23" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M23" s="25" t="s">
         <v>60</v>
       </c>
@@ -4544,7 +4579,9 @@
         <v>60</v>
       </c>
       <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="L24" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M24" s="25" t="s">
         <v>60</v>
       </c>
@@ -4674,7 +4711,9 @@
         <v>60</v>
       </c>
       <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
+      <c r="L27" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="M27" s="25" t="s">
         <v>60</v>
       </c>
@@ -14351,7 +14390,7 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="25" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Aggiornata checklist con chiarimenti su test id=45
GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB/1.1.2/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\FSE test Infosys LDO New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B41C52-2C2C-446D-AFFA-E6E19758C4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29098FCB-43F2-427A-9764-6E8ADDB2744E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="150">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.9.2.180914.2934d0630f94453fe6d101e49a0a45fd5dbf1c4fb3a7571e5a9ea898f5f738e2.209a55cdea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>In caso di timeout l'utente viene invitato a riprovare ad effettuare la validazione e firma del referto, e se il problema persiste ad aprire un ticket di supporto sulla piattaforma helpdesk. Una volta risolta l'anomalia la validazione verrà effettuata manualmente da un operatore in backoffice ed il documento potrà quindi essere firmato e processato.</t>
   </si>
 </sst>
 </file>
@@ -3589,8 +3592,8 @@
   <dimension ref="A1:T656"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O16" sqref="O16"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -4109,7 +4112,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="75.75" thickBot="1">
+    <row r="16" spans="1:20" ht="195.75" thickBot="1">
       <c r="A16" s="20">
         <v>45</v>
       </c>
@@ -4143,10 +4146,10 @@
         <v>116</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="P16" s="32" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>

</xml_diff>